<commit_message>
feat: Kapitel 4 Excel und 04_01  Abbildung erneuert
</commit_message>
<xml_diff>
--- a/Excel/04_01_Quantitative Analyse.xlsx
+++ b/Excel/04_01_Quantitative Analyse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bosch-my.sharepoint.com/personal/nnr3fe_bosch_com/Documents/PersonalDrive/HTWG/BA/LaTex/Thesis/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{0C597558-2E63-CA49-840B-9BE85485DBEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E80E63A7-6714-4483-AC17-B091554F4728}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{0C597558-2E63-CA49-840B-9BE85485DBEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92BF4D15-710F-4DCA-A432-2CFC7258AAD9}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jahr" sheetId="8" r:id="rId1"/>
@@ -207,9 +207,6 @@
     <t>Ensemble &amp; Baum-basiert</t>
   </si>
   <si>
-    <t>P1, P2, P3, P4, P5, P6, P7, P8, P10, P11, P12, P13, P14, P15, P16, P17, P19, P20</t>
-  </si>
-  <si>
     <t>P1, P3, P8, P11,  P12, P14, P20</t>
   </si>
   <si>
@@ -237,12 +234,6 @@
     <t>P5, P15</t>
   </si>
   <si>
-    <t>21/21</t>
-  </si>
-  <si>
-    <t>19/21</t>
-  </si>
-  <si>
     <t>P7, P13</t>
   </si>
   <si>
@@ -297,16 +288,7 @@
     <t>P3, P12, P14</t>
   </si>
   <si>
-    <t>P2, P6, P8, P11, P15, P17, P20, P21</t>
-  </si>
-  <si>
     <t>Klassische Klassifikation/ Regression</t>
-  </si>
-  <si>
-    <t>P3, P4, P6, P7, P8, P9, P10, P14, P19, P20</t>
-  </si>
-  <si>
-    <t>P3, P4, P6, P8, P12, P14, P20</t>
   </si>
   <si>
     <r>
@@ -667,12 +649,6 @@
     <t>Optimierung von CI/CD-Pipelines</t>
   </si>
   <si>
-    <t>Resilienz, Self-Healing und Predictive Maintenance</t>
-  </si>
-  <si>
-    <t>Intelligente Bereitstellung (Edge-AI &amp; Serverless)</t>
-  </si>
-  <si>
     <t xml:space="preserve">AI Governance, Datenschutz und Compliance </t>
   </si>
   <si>
@@ -682,9 +658,6 @@
     <t xml:space="preserve">Datenqualität, Datenverfügbarkeit und Heterogenität </t>
   </si>
   <si>
-    <t>P1, P2, P5,P8, P9, P13, P15,  P16, P17, P20, P21</t>
-  </si>
-  <si>
     <t>Erwähnt</t>
   </si>
   <si>
@@ -707,6 +680,33 @@
   </si>
   <si>
     <t>Erwähnt = lediglich erwähnt, ohne inhaltliche Ausführung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Betrieb &amp; Orchestrierung </t>
+  </si>
+  <si>
+    <t xml:space="preserve">P5 </t>
+  </si>
+  <si>
+    <t>17/18</t>
+  </si>
+  <si>
+    <t>15/18</t>
+  </si>
+  <si>
+    <t>P1, P2, P8, P9, P13, P15,  P16, P17, P20, P21</t>
+  </si>
+  <si>
+    <t>P2,  P8, P11, P15, P17, P20, P21</t>
+  </si>
+  <si>
+    <t>P1, P2, P3, P4, P5, P8, P10, P11, P12, P13, P14, P15, P16, P17, P19, P20</t>
+  </si>
+  <si>
+    <t>P3, P4, P8, P9, P10, P14, P19, P20</t>
+  </si>
+  <si>
+    <t>P3, P4, P8, P12, P14, P20</t>
   </si>
 </sst>
 </file>
@@ -1835,9 +1835,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFB2BFCE"/>
       <color rgb="FF66D0C6"/>
       <color rgb="FF00B1A0"/>
-      <color rgb="FFB2BFCE"/>
       <color rgb="FF334152"/>
       <color rgb="FF546B86"/>
     </mruColors>
@@ -1990,13 +1990,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>5</c:v>
@@ -2067,9 +2067,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2256,16 +2253,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -2357,7 +2351,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -2550,19 +2544,19 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.95238095238095233</c:v>
+                  <c:v>0.94444444444444442</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.90476190476190477</c:v>
+                  <c:v>0.83333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.80952380952380953</c:v>
+                  <c:v>0.83333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.80952380952380953</c:v>
+                  <c:v>0.77777777777777779</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.7142857142857143</c:v>
+                  <c:v>0.72222222222222221</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2863,7 +2857,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="66D0C6"/>
+                <a:srgbClr val="B2BFCE"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -2923,7 +2917,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:srgbClr val="66D0C6"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -2938,31 +2932,11 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="B2BFCE"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000009-3501-4B2E-91D3-558D5FBFB45B}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>'Use cases'!$E$2:$E$6</c:f>
+              <c:f>'Use cases'!$E$2:$E$5</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Optimierung von CI/CD-Pipelines</c:v>
                 </c:pt>
@@ -2973,34 +2947,28 @@
                   <c:v>Sicherheits- &amp; Bedrohungserkennung</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Resilienz, Self-Healing und Predictive Maintenance</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Intelligente Bereitstellung (Edge-AI &amp; Serverless)</c:v>
+                  <c:v>Betrieb &amp; Orchestrierung </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Use cases'!$F$2:$F$6</c:f>
+              <c:f>'Use cases'!$F$2:$F$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3314,10 +3282,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -3747,13 +3715,13 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.8571428571428571</c:v>
+                  <c:v>0.88888888888888884</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.33333333333333331</c:v>
+                  <c:v>0.3888888888888889</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.52380952380952384</c:v>
+                  <c:v>0.44444444444444442</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.33333333333333331</c:v>
@@ -7192,7 +7160,7 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7210,16 +7178,16 @@
         <v>10</v>
       </c>
       <c r="B1" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="24" t="s">
         <v>69</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>72</v>
       </c>
       <c r="F1" s="19"/>
     </row>
@@ -7228,7 +7196,7 @@
         <v>2021</v>
       </c>
       <c r="B2" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
@@ -7250,7 +7218,7 @@
         <v>2023</v>
       </c>
       <c r="B4" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="2"/>
@@ -7263,9 +7231,7 @@
       <c r="B5" s="18">
         <v>5</v>
       </c>
-      <c r="C5" s="18">
-        <v>1</v>
-      </c>
+      <c r="C5" s="18"/>
       <c r="D5" s="2">
         <v>1</v>
       </c>
@@ -7355,8 +7321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24799D05-FC12-4E10-8DB7-F9A31CAD1DF2}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView topLeftCell="C7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7395,10 +7361,10 @@
         <v>32</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="F2" s="32">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -7415,7 +7381,7 @@
         <v>21</v>
       </c>
       <c r="F3" s="32">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -7432,12 +7398,12 @@
         <v>22</v>
       </c>
       <c r="F4" s="32">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>28</v>
@@ -7446,15 +7412,15 @@
         <v>34</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="F5" s="32">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>28</v>
@@ -7462,25 +7428,21 @@
       <c r="C6" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="35" t="s">
-        <v>145</v>
-      </c>
-      <c r="F6" s="36">
-        <v>4</v>
-      </c>
+      <c r="E6" s="35"/>
+      <c r="F6" s="36"/>
     </row>
     <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E10" s="38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F10" s="39" t="s">
         <v>7</v>
@@ -7488,90 +7450,92 @@
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="2"/>
+        <v>151</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>150</v>
+      </c>
       <c r="E11" s="48" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F11" s="41">
-        <f xml:space="preserve"> 20/21</f>
-        <v>0.95238095238095233</v>
+        <f xml:space="preserve"> 17/18</f>
+        <v>0.94444444444444442</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>64</v>
+        <v>152</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E12" s="49" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F12" s="41">
-        <f xml:space="preserve"> 19/21</f>
-        <v>0.90476190476190477</v>
+        <f xml:space="preserve"> 15/18</f>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>64</v>
+        <v>152</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E13" s="49" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F13" s="41">
-        <f xml:space="preserve"> 17/21</f>
-        <v>0.80952380952380953</v>
+        <f xml:space="preserve"> 15/18</f>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E14" s="49" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="F14" s="41">
-        <f xml:space="preserve"> 17/21</f>
-        <v>0.80952380952380953</v>
+        <f xml:space="preserve"> 14/18</f>
+        <v>0.77777777777777779</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>50</v>
       </c>
       <c r="E15" s="50" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="F15" s="42">
-        <f xml:space="preserve"> 15/21</f>
-        <v>0.7142857142857143</v>
+        <f xml:space="preserve"> 13/18</f>
+        <v>0.72222222222222221</v>
       </c>
     </row>
   </sheetData>
@@ -7589,8 +7553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B6F798B-F129-4C52-8944-FD82D34941C3}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView topLeftCell="A3" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7605,22 +7569,22 @@
         <v>19</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="C1" s="51" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D1" s="52" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -7631,19 +7595,19 @@
         <v>6</v>
       </c>
       <c r="C2" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1">
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -7654,16 +7618,16 @@
         <v>3</v>
       </c>
       <c r="C3" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>83</v>
+        <v>154</v>
       </c>
       <c r="G3" s="2"/>
     </row>
@@ -7681,11 +7645,11 @@
         <v>4</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="2" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -7702,8 +7666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F08444-4000-4A0F-9CD0-9E41C62F8163}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7730,11 +7694,11 @@
         <v>51</v>
       </c>
       <c r="B2" s="45">
-        <f xml:space="preserve"> 18/21</f>
-        <v>0.8571428571428571</v>
+        <f xml:space="preserve"> 16/18</f>
+        <v>0.88888888888888884</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>53</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -7742,23 +7706,23 @@
         <v>52</v>
       </c>
       <c r="B3" s="45">
-        <f>7/21</f>
-        <v>0.33333333333333331</v>
+        <f>7/18</f>
+        <v>0.3888888888888889</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="37" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B4" s="45">
-        <f>11/21</f>
-        <v>0.52380952380952384</v>
+        <f>8/18</f>
+        <v>0.44444444444444442</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>85</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -7766,11 +7730,11 @@
         <v>49</v>
       </c>
       <c r="B5" s="46">
-        <f>7/21</f>
+        <f>6/18</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>86</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -7798,198 +7762,198 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="43" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B1" s="43" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C1" s="43" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D1" s="43" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="43" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B2" s="44" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D2" s="44" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="43" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D3" s="44" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="43" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B4" s="44" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D4" s="44" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="43" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D5" s="44" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="43" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B6" s="44" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D6" s="44" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="43" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B7" s="44" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D7" s="44" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="43" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B8" s="44" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D8" s="44" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="43" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B9" s="44" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C9" s="44" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D9" s="44" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="43" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B10" s="44" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D10" s="44" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="43" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B11" s="44" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C11" s="44" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D11" s="44" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="43" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B12" s="44" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C12" s="44" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D12" s="44" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="43" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B13" s="44" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C13" s="44" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D13" s="44" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="43" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B14" s="44" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C14" s="44" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D14" s="44" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -8025,10 +7989,10 @@
         <v>22</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F1" s="47" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G1" s="9"/>
     </row>
@@ -8085,7 +8049,7 @@
     </row>
     <row r="7" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="29" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -8096,7 +8060,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="29" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -8126,12 +8090,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="53" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
feat: 04_01 komplett überarbeitet
</commit_message>
<xml_diff>
--- a/Excel/04_01_Quantitative Analyse.xlsx
+++ b/Excel/04_01_Quantitative Analyse.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bosch-my.sharepoint.com/personal/nnr3fe_bosch_com/Documents/PersonalDrive/HTWG/BA/LaTex/Thesis/Excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nilsarnold/Documents/WIN-Studium/7. Semester/BA/Thesis/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{0C597558-2E63-CA49-840B-9BE85485DBEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92BF4D15-710F-4DCA-A432-2CFC7258AAD9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBAABCE-9121-3E48-8D03-5446DCE226EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jahr" sheetId="8" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="157">
   <si>
     <t>5x</t>
   </si>
@@ -238,12 +238,6 @@
   </si>
   <si>
     <t>P3, P4, P5, P7, P8, P13</t>
-  </si>
-  <si>
-    <t>20/21</t>
-  </si>
-  <si>
-    <t>15/21</t>
   </si>
   <si>
     <t>Journal</t>
@@ -707,6 +701,9 @@
   </si>
   <si>
     <t>P3, P4, P8, P12, P14, P20</t>
+  </si>
+  <si>
+    <t>13/18</t>
   </si>
 </sst>
 </file>
@@ -2366,6 +2363,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2373,7 +2371,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3028,6 +3025,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -3035,7 +3033,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3217,7 +3214,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3</c:v>
@@ -3282,7 +3279,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>7</c:v>
@@ -3529,6 +3526,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -3536,7 +3534,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -7163,35 +7160,35 @@
       <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.81640625" customWidth="1"/>
-    <col min="2" max="3" width="21.453125" customWidth="1"/>
-    <col min="4" max="4" width="25.1796875" customWidth="1"/>
-    <col min="5" max="5" width="27.6328125" customWidth="1"/>
-    <col min="6" max="7" width="21.453125" customWidth="1"/>
-    <col min="8" max="8" width="27.6328125" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="3" width="21.5" customWidth="1"/>
+    <col min="4" max="4" width="25.1640625" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" customWidth="1"/>
+    <col min="6" max="7" width="21.5" customWidth="1"/>
+    <col min="8" max="8" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="E1" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>69</v>
-      </c>
       <c r="F1" s="19"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="20">
         <v>2021</v>
       </c>
@@ -7202,7 +7199,7 @@
       <c r="D2" s="18"/>
       <c r="E2" s="21"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="20">
         <v>2022</v>
       </c>
@@ -7213,7 +7210,7 @@
       <c r="D3" s="16"/>
       <c r="E3" s="21"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="20">
         <v>2023</v>
       </c>
@@ -7224,7 +7221,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="21"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="20">
         <v>2024</v>
       </c>
@@ -7239,7 +7236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="25">
         <v>2025</v>
       </c>
@@ -7252,57 +7249,57 @@
       <c r="D6" s="27"/>
       <c r="E6" s="28"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="17"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="17"/>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="17"/>
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="17"/>
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="17"/>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="17"/>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="17"/>
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="17"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -7321,19 +7318,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24799D05-FC12-4E10-8DB7-F9A31CAD1DF2}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.36328125" customWidth="1"/>
-    <col min="2" max="2" width="17.453125" customWidth="1"/>
-    <col min="3" max="3" width="37.81640625" customWidth="1"/>
-    <col min="5" max="6" width="23.1796875" style="30" customWidth="1"/>
+    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="37.83203125" customWidth="1"/>
+    <col min="5" max="6" width="23.1640625" style="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>18</v>
       </c>
@@ -7350,7 +7347,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>20</v>
       </c>
@@ -7361,13 +7358,13 @@
         <v>32</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F2" s="32">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>21</v>
       </c>
@@ -7384,7 +7381,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>22</v>
       </c>
@@ -7401,9 +7398,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>28</v>
@@ -7412,15 +7409,15 @@
         <v>34</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F5" s="32">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>28</v>
@@ -7431,7 +7428,7 @@
       <c r="E6" s="35"/>
       <c r="F6" s="36"/>
     </row>
-    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>54</v>
       </c>
@@ -7448,15 +7445,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E11" s="48" t="s">
         <v>57</v>
@@ -7466,12 +7463,12 @@
         <v>0.94444444444444442</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>61</v>
@@ -7484,54 +7481,54 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E13" s="49" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F13" s="41">
         <f xml:space="preserve"> 15/18</f>
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>65</v>
+        <v>150</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>63</v>
       </c>
       <c r="E14" s="49" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F14" s="41">
         <f xml:space="preserve"> 14/18</f>
         <v>0.77777777777777779</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>64</v>
+        <v>156</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>50</v>
       </c>
       <c r="E15" s="50" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F15" s="42">
         <f xml:space="preserve"> 13/18</f>
@@ -7553,64 +7550,64 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B6F798B-F129-4C52-8944-FD82D34941C3}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView zoomScale="84" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="17.81640625" customWidth="1"/>
-    <col min="5" max="6" width="32.6328125" customWidth="1"/>
-    <col min="7" max="7" width="19.81640625" customWidth="1"/>
+    <col min="1" max="4" width="17.83203125" customWidth="1"/>
+    <col min="5" max="6" width="32.6640625" customWidth="1"/>
+    <col min="7" max="7" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1" s="51" t="s">
+        <v>145</v>
+      </c>
+      <c r="D1" s="52" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="51" t="s">
-        <v>147</v>
-      </c>
-      <c r="D1" s="52" t="s">
-        <v>148</v>
-      </c>
       <c r="E1" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1">
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -7624,14 +7621,14 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -7645,11 +7642,11 @@
         <v>4</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -7666,19 +7663,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F08444-4000-4A0F-9CD0-9E41C62F8163}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="32.1796875" customWidth="1"/>
-    <col min="3" max="3" width="34.81640625" customWidth="1"/>
-    <col min="4" max="4" width="47.6328125" customWidth="1"/>
-    <col min="5" max="6" width="26.1796875" customWidth="1"/>
+    <col min="1" max="2" width="32.1640625" customWidth="1"/>
+    <col min="3" max="3" width="34.83203125" customWidth="1"/>
+    <col min="4" max="4" width="47.6640625" customWidth="1"/>
+    <col min="5" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="38" t="s">
         <v>12</v>
       </c>
@@ -7689,7 +7686,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="37" t="s">
         <v>51</v>
       </c>
@@ -7698,10 +7695,10 @@
         <v>0.88888888888888884</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="37" t="s">
         <v>52</v>
       </c>
@@ -7713,19 +7710,19 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="37" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B4" s="45">
         <f>8/18</f>
         <v>0.44444444444444442</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="40" t="s">
         <v>49</v>
       </c>
@@ -7734,7 +7731,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -7755,205 +7752,205 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="28.6328125" customWidth="1"/>
+    <col min="1" max="4" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="D1" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="43" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="B2" s="44" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="43" t="s">
+      <c r="C2" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="D2" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="C2" s="44" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="B3" s="44" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="43" t="s">
+      <c r="C3" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="D3" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="44" t="s">
+    </row>
+    <row r="4" spans="1:4" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="B4" s="44" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="43" t="s">
+      <c r="C4" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="D4" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="44" t="s">
+    </row>
+    <row r="5" spans="1:4" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="D4" s="44" t="s">
+      <c r="B5" s="44" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="43" t="s">
+      <c r="C5" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="D5" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="C5" s="44" t="s">
+    </row>
+    <row r="6" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="D5" s="44" t="s">
+      <c r="B6" s="44" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="43" t="s">
+      <c r="C6" s="44" t="s">
         <v>101</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="D6" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="C6" s="44" t="s">
+    </row>
+    <row r="7" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="D6" s="44" t="s">
+      <c r="B7" s="44" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="43" t="s">
+      <c r="C7" s="44" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="D7" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="C7" s="44" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="43" t="s">
         <v>107</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="B8" s="44" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="43" t="s">
+      <c r="C8" s="44" t="s">
         <v>109</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="D8" s="44" t="s">
         <v>110</v>
       </c>
-      <c r="C8" s="44" t="s">
+    </row>
+    <row r="9" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="D8" s="44" t="s">
+      <c r="B9" s="44" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="43" t="s">
+      <c r="C9" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="D9" s="44" t="s">
         <v>114</v>
       </c>
-      <c r="C9" s="44" t="s">
+    </row>
+    <row r="10" spans="1:4" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="D9" s="44" t="s">
+      <c r="B10" s="44" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="43" t="s">
+      <c r="C10" s="44" t="s">
         <v>117</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="D10" s="44" t="s">
         <v>118</v>
       </c>
-      <c r="C10" s="44" t="s">
+    </row>
+    <row r="11" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="D10" s="44" t="s">
+      <c r="B11" s="44" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="43" t="s">
+      <c r="C11" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="B11" s="44" t="s">
+      <c r="D11" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="C11" s="44" t="s">
+    </row>
+    <row r="12" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="D11" s="44" t="s">
+      <c r="B12" s="44" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="43" t="s">
+      <c r="C12" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="D12" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="C12" s="44" t="s">
+    </row>
+    <row r="13" spans="1:4" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="43" t="s">
         <v>127</v>
       </c>
-      <c r="D12" s="44" t="s">
+      <c r="B13" s="44" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="43" t="s">
+      <c r="C13" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="B13" s="44" t="s">
+      <c r="D13" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="C13" s="44" t="s">
+    </row>
+    <row r="14" spans="1:4" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="43" t="s">
         <v>131</v>
       </c>
-      <c r="D13" s="44" t="s">
+      <c r="B14" s="44" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="43" t="s">
+      <c r="C14" s="44" t="s">
         <v>133</v>
       </c>
-      <c r="B14" s="44" t="s">
+      <c r="D14" s="44" t="s">
         <v>134</v>
-      </c>
-      <c r="C14" s="44" t="s">
-        <v>135</v>
-      </c>
-      <c r="D14" s="44" t="s">
-        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -7970,12 +7967,12 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="7" width="25.81640625" customWidth="1"/>
+    <col min="1" max="7" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>17</v>
       </c>
@@ -7989,14 +7986,14 @@
         <v>22</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="47" t="s">
-        <v>76</v>
-      </c>
       <c r="G1" s="9"/>
     </row>
-    <row r="2" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>16</v>
       </c>
@@ -8006,7 +8003,7 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>15</v>
       </c>
@@ -8016,7 +8013,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>14</v>
       </c>
@@ -8026,7 +8023,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>13</v>
       </c>
@@ -8036,7 +8033,7 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="29" t="s">
         <v>52</v>
       </c>
@@ -8047,9 +8044,9 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -8058,9 +8055,9 @@
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -8083,73 +8080,73 @@
       <selection activeCell="A2" sqref="A2:A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="113.453125" customWidth="1"/>
+    <col min="1" max="1" width="113.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="53" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="53"/>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="53"/>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="53"/>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="53"/>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="53"/>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="53"/>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="53"/>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="53"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="53"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="53"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="53"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="53"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="53"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" s="53"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="53"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="53"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="53"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="53"/>
     </row>
   </sheetData>
@@ -8169,18 +8166,18 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="37.81640625" customWidth="1"/>
+    <col min="1" max="3" width="37.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="10"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
@@ -8191,7 +8188,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -8202,7 +8199,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -8213,7 +8210,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -8224,7 +8221,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -8235,7 +8232,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -8246,7 +8243,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
@@ -8257,13 +8254,13 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
         <v>24</v>
       </c>
       <c r="B10" s="10"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
@@ -8274,7 +8271,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -8285,7 +8282,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
@@ -8296,7 +8293,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -8307,7 +8304,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>9</v>
       </c>
@@ -8318,7 +8315,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
@@ -8329,7 +8326,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
feat. Excel Dateien erweitert
</commit_message>
<xml_diff>
--- a/Excel/04_01_Quantitative Analyse.xlsx
+++ b/Excel/04_01_Quantitative Analyse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nilsarnold/Documents/WIN-Studium/7. Semester/BA/Thesis/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBAABCE-9121-3E48-8D03-5446DCE226EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F3F297-A2D6-4245-85F1-6403B21532F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jahr" sheetId="8" r:id="rId1"/>
@@ -643,9 +643,6 @@
     <t>Optimierung von CI/CD-Pipelines</t>
   </si>
   <si>
-    <t xml:space="preserve">AI Governance, Datenschutz und Compliance </t>
-  </si>
-  <si>
     <t xml:space="preserve">Integrationskomplexität &amp; Abhängigkeiten </t>
   </si>
   <si>
@@ -704,6 +701,9 @@
   </si>
   <si>
     <t>13/18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KI-Governance, Datenschutz und Compliance </t>
   </si>
 </sst>
 </file>
@@ -2523,7 +2523,7 @@
                   <c:v>Skalierbarkeit, Latenz &amp; Monitoring</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>AI Governance, Datenschutz und Compliance </c:v>
+                  <c:v>KI-Governance, Datenschutz und Compliance </c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Integrationskomplexität &amp; Abhängigkeiten </c:v>
@@ -7318,8 +7318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24799D05-FC12-4E10-8DB7-F9A31CAD1DF2}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:B15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7409,7 +7409,7 @@
         <v>34</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F5" s="32">
         <v>5</v>
@@ -7450,10 +7450,10 @@
         <v>57</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E11" s="48" t="s">
         <v>57</v>
@@ -7468,7 +7468,7 @@
         <v>58</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>61</v>
@@ -7481,18 +7481,18 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E13" s="49" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="F13" s="41">
         <f xml:space="preserve"> 15/18</f>
@@ -7504,13 +7504,13 @@
         <v>55</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>63</v>
       </c>
       <c r="E14" s="49" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F14" s="41">
         <f xml:space="preserve"> 14/18</f>
@@ -7522,13 +7522,13 @@
         <v>60</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>50</v>
       </c>
       <c r="E15" s="50" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F15" s="42">
         <f xml:space="preserve"> 13/18</f>
@@ -7566,13 +7566,13 @@
         <v>19</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" s="51" t="s">
         <v>144</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="D1" s="52" t="s">
         <v>145</v>
-      </c>
-      <c r="D1" s="52" t="s">
-        <v>146</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>75</v>
@@ -7581,7 +7581,7 @@
         <v>76</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -7598,13 +7598,13 @@
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -7624,7 +7624,7 @@
         <v>77</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G3" s="2"/>
     </row>
@@ -7642,11 +7642,11 @@
         <v>4</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -7663,8 +7663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F08444-4000-4A0F-9CD0-9E41C62F8163}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7695,7 +7695,7 @@
         <v>0.88888888888888884</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -7719,7 +7719,7 @@
         <v>0.44444444444444442</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -7731,7 +7731,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Excel und Abbildung 04_03_01
</commit_message>
<xml_diff>
--- a/Excel/04_01_Quantitative Analyse.xlsx
+++ b/Excel/04_01_Quantitative Analyse.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10102"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nilsarnold/Documents/WIN-Studium/7. Semester/BA/Thesis/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F3F297-A2D6-4245-85F1-6403B21532F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D310E3C-4A76-9C4B-A6BC-AE3E46C7DAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jahr" sheetId="8" r:id="rId1"/>
@@ -6754,13 +6754,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>55562</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>11112</xdr:rowOff>
+      <xdr:rowOff>11113</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>301625</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1451428</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>136072</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7318,7 +7318,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24799D05-FC12-4E10-8DB7-F9A31CAD1DF2}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
@@ -7481,7 +7481,7 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>59</v>
       </c>
@@ -7550,8 +7550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B6F798B-F129-4C52-8944-FD82D34941C3}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView zoomScale="84" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>